<commit_message>
fixed package errors and added requirements.txt
</commit_message>
<xml_diff>
--- a/example/compounds.xlsx
+++ b/example/compounds.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longd\OneDrive - The University of Auckland\Documents\UoA Research\MS_Research\MS-Binding-Sites-Identification\src\defaults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\longd\OneDrive - The University of Auckland\Documents\UoA Research\MS_Research\MS-Binding-Sites-Identification\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E898E4B-17F3-4A96-94BF-E137160BE787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE781E3F-B308-412A-907A-7668659AC186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>